<commit_message>
animation and dialogue Bug fixed
</commit_message>
<xml_diff>
--- a/GameDesign/ExcelData/Dialogue_Data.xlsx
+++ b/GameDesign/ExcelData/Dialogue_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\University\ucsc\GAME 271\project-Nameless Hill\NamelessHill_Temp\Nameless_Temp\GameDesign\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27BB6624-14CB-421F-AA7D-F1AB08F70B20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D70FA84-30CC-4116-8F6E-61D8EEC4738F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -430,7 +430,7 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="F3" sqref="F3:F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -524,10 +524,10 @@
         <v>3</v>
       </c>
       <c r="F3" s="1">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="G3" s="1">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="H3" s="1">
         <v>3</v>
@@ -556,10 +556,10 @@
         <v>3</v>
       </c>
       <c r="F4" s="1">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="G4" s="1">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="H4" s="1">
         <v>3</v>
@@ -588,10 +588,10 @@
         <v>3</v>
       </c>
       <c r="F5" s="1">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="G5" s="1">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="H5" s="1">
         <v>3</v>
@@ -620,10 +620,10 @@
         <v>3</v>
       </c>
       <c r="F6" s="1">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="G6" s="1">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="H6" s="1">
         <v>3</v>
@@ -652,10 +652,10 @@
         <v>3</v>
       </c>
       <c r="F7" s="1">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="G7" s="1">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="H7" s="1">
         <v>3</v>
@@ -684,10 +684,10 @@
         <v>3</v>
       </c>
       <c r="F8" s="1">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="G8" s="1">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="H8" s="1">
         <v>3</v>
@@ -716,10 +716,10 @@
         <v>3</v>
       </c>
       <c r="F9" s="1">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="G9" s="1">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="H9" s="1">
         <v>3</v>

</xml_diff>